<commit_message>
Rajout de la colonne Habitat dans les .xlsx. + Modifications de Carnet.Rnw, Carnet.Rmd, Agregplacettes pour qu'ils prennent en compte les TarifIIFN + Modifications sur Verif.R (format pdf fonctionne) et ClasseurRem (choix de plusieurs réserves en même temps + Dans PsdrfCarnetVal.Rmd, j'ai ajouté un bouton tcl pour contourner l'absence de données SIG (cela a entrainé quelques adaptations en +)
</commit_message>
<xml_diff>
--- a/Data/Export/10 RB Glaciere.xlsx
+++ b/Data/Export/10 RB Glaciere.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Placettes" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Arbres!$A$1:$Q$1504</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Placettes!$A$1:$Q$45</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="114210" iterateDelta="1E-4" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10125" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10126" uniqueCount="509">
   <si>
     <t>num</t>
   </si>
@@ -1554,28 +1549,29 @@
   <si>
     <t>Groupe2</t>
   </si>
+  <si>
+    <t>Habitat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1584,7 +1580,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1593,27 +1589,17 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1638,19 +1624,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor indexed="13"/>
+        <bgColor indexed="8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor indexed="22"/>
+        <bgColor indexed="8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor indexed="55"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,8 +1650,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -1675,77 +1671,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="16">
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+  <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="6"/>
-    <cellStyle name="Normal 3" xfId="8"/>
-    <cellStyle name="Normal 4" xfId="15"/>
-    <cellStyle name="Pourcentage 2" xfId="7"/>
-    <cellStyle name="XLConnect.Boolean" xfId="4"/>
-    <cellStyle name="XLConnect.DateTime" xfId="5"/>
-    <cellStyle name="XLConnect.Header" xfId="1"/>
-    <cellStyle name="XLConnect.Numeric" xfId="3"/>
-    <cellStyle name="XLConnect.String" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Pourcentage 2" xfId="4"/>
+    <cellStyle name="XLConnect.Boolean" xfId="5"/>
+    <cellStyle name="XLConnect.DateTime" xfId="6"/>
+    <cellStyle name="XLConnect.Header" xfId="7"/>
+    <cellStyle name="XLConnect.Numeric" xfId="8"/>
+    <cellStyle name="XLConnect.String" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2035,18 +2002,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2780" topLeftCell="A38"/>
-      <selection activeCell="R1" sqref="R1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2775" topLeftCell="A38"/>
+      <selection activeCell="T2" sqref="T2"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="5" t="s">
         <v>499</v>
       </c>
@@ -2104,8 +2071,11 @@
       <c r="S1" s="11" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="5" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -2155,7 +2125,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" s="3">
         <v>10</v>
       </c>
@@ -2205,7 +2175,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>10</v>
       </c>
@@ -2255,7 +2225,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="3">
         <v>10</v>
       </c>
@@ -2305,7 +2275,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="3">
         <v>10</v>
       </c>
@@ -2355,7 +2325,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="3">
         <v>10</v>
       </c>
@@ -2405,7 +2375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" s="3">
         <v>10</v>
       </c>
@@ -2455,7 +2425,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -2505,7 +2475,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -2555,7 +2525,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2605,7 +2575,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2655,7 +2625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2705,7 +2675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -2755,7 +2725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -2805,7 +2775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="3">
         <v>10</v>
       </c>
@@ -4307,30 +4277,23 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q45"/>
-  <sortState ref="A2:V45">
-    <sortCondition ref="B2:B45"/>
-  </sortState>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q1504"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1660" topLeftCell="A1504"/>
+      <pane ySplit="1665" topLeftCell="A1504"/>
       <selection activeCell="D3" sqref="D3:D1504"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="5" t="s">
@@ -70225,29 +70188,20 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q1504">
-    <sortCondition ref="A2:A1504"/>
-    <sortCondition ref="B2:B1504"/>
-    <sortCondition ref="F2:F1504"/>
-  </sortState>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:A65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
@@ -87570,24 +87524,20 @@
       <c r="M444" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:A65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
@@ -96560,27 +96510,23 @@
       <c r="L249" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="J2:K249" numberStoredAsText="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:A65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="11" t="s">
@@ -103569,27 +103515,23 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="K2:L146" numberStoredAsText="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
@@ -103615,796 +103557,788 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>504</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="1" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="14">
-        <v>10</v>
-      </c>
-      <c r="B2" s="14">
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <v>40729</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="14">
-        <v>10</v>
-      </c>
-      <c r="B3" s="14">
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" s="13">
         <v>1</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="16">
         <v>40729</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="14">
-        <v>10</v>
-      </c>
-      <c r="B4" s="14">
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="3">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>40724</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="14">
-        <v>10</v>
-      </c>
-      <c r="B5" s="14">
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="3">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="16">
         <v>40724</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="14">
-        <v>10</v>
-      </c>
-      <c r="B6" s="14">
+    <row r="6" spans="1:5" ht="15.75">
+      <c r="A6" s="3">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
         <v>5</v>
       </c>
       <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="14">
-        <v>10</v>
-      </c>
-      <c r="B7" s="14">
+    <row r="7" spans="1:5" ht="15.75">
+      <c r="A7" s="3">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
         <v>6</v>
       </c>
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="14">
-        <v>10</v>
-      </c>
-      <c r="B8" s="14">
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="A8" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
         <v>7</v>
       </c>
       <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>40729</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="14">
-        <v>10</v>
-      </c>
-      <c r="B9" s="14">
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <v>40724</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="14">
-        <v>10</v>
-      </c>
-      <c r="B10" s="14">
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
         <v>9</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>40729</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14">
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <v>40668</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="14">
-        <v>10</v>
-      </c>
-      <c r="B12" s="14">
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
         <v>11</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>40668</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="14">
-        <v>10</v>
-      </c>
-      <c r="B13" s="14">
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
         <v>12</v>
       </c>
       <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="14">
-        <v>10</v>
-      </c>
-      <c r="B14" s="14">
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
         <v>13</v>
       </c>
       <c r="C14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="3">
         <v>3</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="14">
-        <v>10</v>
-      </c>
-      <c r="B15" s="14">
+    <row r="15" spans="1:5" ht="15.75">
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
         <v>14</v>
       </c>
       <c r="C15" s="13">
         <v>1</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="3">
         <v>3</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>40724</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="14">
-        <v>10</v>
-      </c>
-      <c r="B16" s="14">
+    <row r="16" spans="1:5" ht="15.75">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3">
         <v>15</v>
       </c>
       <c r="C16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="3">
         <v>3</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <v>40724</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
-      <c r="A17" s="14">
-        <v>10</v>
-      </c>
-      <c r="B17" s="14">
+    <row r="17" spans="1:5" ht="15.75">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
         <v>16</v>
       </c>
       <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="3">
         <v>3</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>39089</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="14">
-        <v>10</v>
-      </c>
-      <c r="B18" s="14">
+    <row r="18" spans="1:5" ht="15.75">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3">
         <v>17</v>
       </c>
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <v>39089</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
-      <c r="A19" s="14">
-        <v>10</v>
-      </c>
-      <c r="B19" s="14">
+    <row r="19" spans="1:5" ht="15.75">
+      <c r="A19" s="3">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3">
         <v>18</v>
       </c>
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="3">
         <v>3</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <v>40667</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="14">
-        <v>10</v>
-      </c>
-      <c r="B20" s="14">
+    <row r="20" spans="1:5" ht="15.75">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
         <v>19</v>
       </c>
       <c r="C20" s="13">
         <v>1</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <v>40667</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="14">
-        <v>10</v>
-      </c>
-      <c r="B21" s="14">
+    <row r="21" spans="1:5" ht="15.75">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3">
         <v>20</v>
       </c>
       <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="3">
         <v>3</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
-      <c r="A22" s="14">
-        <v>10</v>
-      </c>
-      <c r="B22" s="14">
+    <row r="22" spans="1:5" ht="15.75">
+      <c r="A22" s="3">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3">
         <v>21</v>
       </c>
       <c r="C22" s="13">
         <v>1</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15">
-      <c r="A23" s="14">
-        <v>10</v>
-      </c>
-      <c r="B23" s="14">
+    <row r="23" spans="1:5" ht="15.75">
+      <c r="A23" s="3">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3">
         <v>22</v>
       </c>
       <c r="C23" s="13">
         <v>1</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <v>39084</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="14">
-        <v>10</v>
-      </c>
-      <c r="B24" s="14">
+    <row r="24" spans="1:5" ht="15.75">
+      <c r="A24" s="3">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
         <v>23</v>
       </c>
       <c r="C24" s="13">
         <v>1</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="3">
         <v>3</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="16">
         <v>39084</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
-      <c r="A25" s="14">
-        <v>10</v>
-      </c>
-      <c r="B25" s="14">
+    <row r="25" spans="1:5" ht="15.75">
+      <c r="A25" s="3">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3">
         <v>24</v>
       </c>
       <c r="C25" s="13">
         <v>1</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="3">
         <v>3</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <v>39089</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15">
-      <c r="A26" s="14">
-        <v>10</v>
-      </c>
-      <c r="B26" s="14">
+    <row r="26" spans="1:5" ht="15.75">
+      <c r="A26" s="3">
+        <v>10</v>
+      </c>
+      <c r="B26" s="3">
         <v>25</v>
       </c>
       <c r="C26" s="13">
         <v>1</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>39089</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
-      <c r="A27" s="14">
-        <v>10</v>
-      </c>
-      <c r="B27" s="14">
+    <row r="27" spans="1:5" ht="15.75">
+      <c r="A27" s="3">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3">
         <v>26</v>
       </c>
       <c r="C27" s="13">
         <v>1</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="3">
         <v>3</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="16">
         <v>40665</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15">
-      <c r="A28" s="14">
-        <v>10</v>
-      </c>
-      <c r="B28" s="14">
+    <row r="28" spans="1:5" ht="15.75">
+      <c r="A28" s="3">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3">
         <v>27</v>
       </c>
       <c r="C28" s="13">
         <v>1</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="3">
         <v>3</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="16">
         <v>40667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15">
-      <c r="A29" s="14">
-        <v>10</v>
-      </c>
-      <c r="B29" s="14">
+    <row r="29" spans="1:5" ht="15.75">
+      <c r="A29" s="3">
+        <v>10</v>
+      </c>
+      <c r="B29" s="3">
         <v>28</v>
       </c>
       <c r="C29" s="13">
         <v>1</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="3">
         <v>3</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="16">
         <v>40667</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15">
-      <c r="A30" s="14">
-        <v>10</v>
-      </c>
-      <c r="B30" s="14">
+    <row r="30" spans="1:5" ht="15.75">
+      <c r="A30" s="3">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3">
         <v>29</v>
       </c>
       <c r="C30" s="13">
         <v>1</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15">
-      <c r="A31" s="14">
-        <v>10</v>
-      </c>
-      <c r="B31" s="14">
+    <row r="31" spans="1:5" ht="15.75">
+      <c r="A31" s="3">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3">
         <v>30</v>
       </c>
       <c r="C31" s="13">
         <v>1</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="3">
         <v>3</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
-      <c r="A32" s="14">
-        <v>10</v>
-      </c>
-      <c r="B32" s="14">
+    <row r="32" spans="1:5" ht="15.75">
+      <c r="A32" s="3">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
         <v>31</v>
       </c>
       <c r="C32" s="13">
         <v>1</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="3">
         <v>3</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15">
-      <c r="A33" s="14">
-        <v>10</v>
-      </c>
-      <c r="B33" s="14">
+    <row r="33" spans="1:5" ht="15.75">
+      <c r="A33" s="3">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3">
         <v>32</v>
       </c>
       <c r="C33" s="13">
         <v>1</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="3">
         <v>3</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15">
-      <c r="A34" s="14">
-        <v>10</v>
-      </c>
-      <c r="B34" s="14">
+    <row r="34" spans="1:5" ht="15.75">
+      <c r="A34" s="3">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
         <v>33</v>
       </c>
       <c r="C34" s="13">
         <v>1</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="3">
         <v>3</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="16">
         <v>40665</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15">
-      <c r="A35" s="14">
-        <v>10</v>
-      </c>
-      <c r="B35" s="14">
+    <row r="35" spans="1:5" ht="15.75">
+      <c r="A35" s="3">
+        <v>10</v>
+      </c>
+      <c r="B35" s="3">
         <v>34</v>
       </c>
       <c r="C35" s="13">
         <v>1</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="3">
         <v>3</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="16">
         <v>40665</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15">
-      <c r="A36" s="14">
-        <v>10</v>
-      </c>
-      <c r="B36" s="14">
+    <row r="36" spans="1:5" ht="15.75">
+      <c r="A36" s="3">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3">
         <v>35</v>
       </c>
       <c r="C36" s="13">
         <v>1</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="3">
         <v>3</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15">
-      <c r="A37" s="14">
-        <v>10</v>
-      </c>
-      <c r="B37" s="14">
+    <row r="37" spans="1:5" ht="15.75">
+      <c r="A37" s="3">
+        <v>10</v>
+      </c>
+      <c r="B37" s="3">
         <v>36</v>
       </c>
       <c r="C37" s="13">
         <v>1</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="3">
         <v>3</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15">
-      <c r="A38" s="14">
-        <v>10</v>
-      </c>
-      <c r="B38" s="14">
+    <row r="38" spans="1:5" ht="15.75">
+      <c r="A38" s="3">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
         <v>37</v>
       </c>
       <c r="C38" s="13">
         <v>1</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="3">
         <v>3</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="16">
         <v>39083</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15">
-      <c r="A39" s="14">
-        <v>10</v>
-      </c>
-      <c r="B39" s="14">
+    <row r="39" spans="1:5" ht="15.75">
+      <c r="A39" s="3">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3">
         <v>38</v>
       </c>
       <c r="C39" s="13">
         <v>1</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="3">
         <v>3</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="16">
         <v>40669</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15">
-      <c r="A40" s="14">
-        <v>10</v>
-      </c>
-      <c r="B40" s="14">
+    <row r="40" spans="1:5" ht="15.75">
+      <c r="A40" s="3">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
         <v>39</v>
       </c>
       <c r="C40" s="13">
         <v>1</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="3">
         <v>3</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="16">
         <v>40662</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15">
-      <c r="A41" s="14">
-        <v>10</v>
-      </c>
-      <c r="B41" s="14">
+    <row r="41" spans="1:5" ht="15.75">
+      <c r="A41" s="3">
+        <v>10</v>
+      </c>
+      <c r="B41" s="3">
         <v>40</v>
       </c>
       <c r="C41" s="13">
         <v>1</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="3">
         <v>3</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="16">
         <v>40662</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15">
-      <c r="A42" s="14">
-        <v>10</v>
-      </c>
-      <c r="B42" s="14">
+    <row r="42" spans="1:5" ht="15.75">
+      <c r="A42" s="3">
+        <v>10</v>
+      </c>
+      <c r="B42" s="3">
         <v>41</v>
       </c>
       <c r="C42" s="13">
         <v>1</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="3">
         <v>3</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="16">
         <v>40709</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15">
-      <c r="A43" s="14">
-        <v>10</v>
-      </c>
-      <c r="B43" s="14">
+    <row r="43" spans="1:5" ht="15.75">
+      <c r="A43" s="3">
+        <v>10</v>
+      </c>
+      <c r="B43" s="3">
         <v>42</v>
       </c>
       <c r="C43" s="13">
         <v>1</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="3">
         <v>3</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="16">
         <v>40732</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15">
-      <c r="A44" s="14">
-        <v>10</v>
-      </c>
-      <c r="B44" s="14">
+    <row r="44" spans="1:5" ht="15.75">
+      <c r="A44" s="3">
+        <v>10</v>
+      </c>
+      <c r="B44" s="3">
         <v>43</v>
       </c>
       <c r="C44" s="13">
         <v>1</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="3">
         <v>3</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="16">
         <v>40732</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15">
-      <c r="A45" s="14">
-        <v>10</v>
-      </c>
-      <c r="B45" s="14">
+    <row r="45" spans="1:5" ht="15.75">
+      <c r="A45" s="3">
+        <v>10</v>
+      </c>
+      <c r="B45" s="3">
         <v>44</v>
       </c>
       <c r="C45" s="13">
         <v>1</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="3">
         <v>3</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="16">
         <v>40709</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>